<commit_message>
new var test results formated
</commit_message>
<xml_diff>
--- a/eval/results/100ms_results/results.xlsx
+++ b/eval/results/100ms_results/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilja\Real-Time-Offloading-Simulator\eval\results\100ms_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Real-Time-Offloading-Simulator/eval/results/100ms_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F867E0C0-1E1E-4B7E-915B-98052BB92276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88377FEE-9099-E44B-8D96-BC2C1BF34E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35535" yWindow="-2070" windowWidth="28800" windowHeight="15435" activeTab="3"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="196">
   <si>
     <t>client_test_10_1</t>
   </si>
@@ -366,12 +366,258 @@
   </si>
   <si>
     <t>Total Tasks</t>
+  </si>
+  <si>
+    <t>0.6621880998080614</t>
+  </si>
+  <si>
+    <t>0.9942028985507246</t>
+  </si>
+  <si>
+    <t>0.2823081817682326</t>
+  </si>
+  <si>
+    <t>0.09902406238931298</t>
+  </si>
+  <si>
+    <t>0.05247218319533528</t>
+  </si>
+  <si>
+    <t>0.07279693486590039</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>0.031235640022371634</t>
+  </si>
+  <si>
+    <t>0.09887070634482759</t>
+  </si>
+  <si>
+    <t>0.08774044418421054</t>
+  </si>
+  <si>
+    <t>0.0020242914979757085</t>
+  </si>
+  <si>
+    <t>0.0008305962135514274</t>
+  </si>
+  <si>
+    <t>0.10157035659109312</t>
+  </si>
+  <si>
+    <t>0.110825212</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>0.1011047810433145</t>
+  </si>
+  <si>
+    <t>0.8681102362204725</t>
+  </si>
+  <si>
+    <t>0.41672757261316384</t>
+  </si>
+  <si>
+    <t>0.1014681961330724</t>
+  </si>
+  <si>
+    <t>0.04485569518367347</t>
+  </si>
+  <si>
+    <t>0.6586715867158671</t>
+  </si>
+  <si>
+    <t>0.9971988795518207</t>
+  </si>
+  <si>
+    <t>0.2927994778966557</t>
+  </si>
+  <si>
+    <t>0.09852864984403668</t>
+  </si>
+  <si>
+    <t>0.05152399449438202</t>
+  </si>
+  <si>
+    <t>0.07824427480916031</t>
+  </si>
+  <si>
+    <t>0.0337850575541801</t>
+  </si>
+  <si>
+    <t>0.10064989088380952</t>
+  </si>
+  <si>
+    <t>0.09176608212195123</t>
+  </si>
+  <si>
+    <t>0.09906880074849095</t>
+  </si>
+  <si>
+    <t>0.09789893444444445</t>
+  </si>
+  <si>
+    <t>0.832046332046332</t>
+  </si>
+  <si>
+    <t>0.42524230000346314</t>
+  </si>
+  <si>
+    <t>0.09932854239005735</t>
+  </si>
+  <si>
+    <t>0.04381946875870069</t>
+  </si>
+  <si>
+    <t>0.6427221172022685</t>
+  </si>
+  <si>
+    <t>0.9941176470588236</t>
+  </si>
+  <si>
+    <t>0.2781391048857909</t>
+  </si>
+  <si>
+    <t>0.09865636424105462</t>
+  </si>
+  <si>
+    <t>0.05204195703254437</t>
+  </si>
+  <si>
+    <t>0.07509881422924901</t>
+  </si>
+  <si>
+    <t>0.031288546620804984</t>
+  </si>
+  <si>
+    <t>0.09897624378895463</t>
+  </si>
+  <si>
+    <t>0.09159809939473684</t>
+  </si>
+  <si>
+    <t>0.001937984496124031</t>
+  </si>
+  <si>
+    <t>0.0008310445616912888</t>
+  </si>
+  <si>
+    <t>0.09916363544487426</t>
+  </si>
+  <si>
+    <t>0.113775198</t>
+  </si>
+  <si>
+    <t>0.10199199458349704</t>
+  </si>
+  <si>
+    <t>0.8128440366972477</t>
+  </si>
+  <si>
+    <t>0.4455926370222093</t>
+  </si>
+  <si>
+    <t>0.10067083811700182</t>
+  </si>
+  <si>
+    <t>0.045975832203160275</t>
+  </si>
+  <si>
+    <t>0.6742424242424242</t>
+  </si>
+  <si>
+    <t>0.29112100993423684</t>
+  </si>
+  <si>
+    <t>0.10134092160075331</t>
+  </si>
+  <si>
+    <t>0.0543017544241573</t>
+  </si>
+  <si>
+    <t>0.073558648111332</t>
+  </si>
+  <si>
+    <t>0.030419232341949706</t>
+  </si>
+  <si>
+    <t>0.10210344999999998</t>
+  </si>
+  <si>
+    <t>0.09016179383783784</t>
+  </si>
+  <si>
+    <t>0.10178629575296443</t>
+  </si>
+  <si>
+    <t>0.09797360214867618</t>
+  </si>
+  <si>
+    <t>0.8502024291497976</t>
+  </si>
+  <si>
+    <t>0.40497021015328166</t>
+  </si>
+  <si>
+    <t>0.10150897982258064</t>
+  </si>
+  <si>
+    <t>0.045361774726190476</t>
+  </si>
+  <si>
+    <t>0.6822429906542056</t>
+  </si>
+  <si>
+    <t>0.9945205479452055</t>
+  </si>
+  <si>
+    <t>0.2993020056403472</t>
+  </si>
+  <si>
+    <t>0.10116277243470148</t>
+  </si>
+  <si>
+    <t>0.05170229027272728</t>
+  </si>
+  <si>
+    <t>0.07459677419354839</t>
+  </si>
+  <si>
+    <t>0.03047140123770763</t>
+  </si>
+  <si>
+    <t>0.09872654574549099</t>
+  </si>
+  <si>
+    <t>0.08974884697297297</t>
+  </si>
+  <si>
+    <t>0.10100066796787148</t>
+  </si>
+  <si>
+    <t>0.09860298094999999</t>
+  </si>
+  <si>
+    <t>0.8065693430656934</t>
+  </si>
+  <si>
+    <t>0.4500761902829683</t>
+  </si>
+  <si>
+    <t>0.09919347464727271</t>
+  </si>
+  <si>
+    <t>0.04256668745701357</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -853,48 +1099,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -910,7 +1156,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1205,16 +1451,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView topLeftCell="A65" workbookViewId="0">
       <selection activeCell="A76" sqref="A76:H100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>10</v>
       </c>
@@ -1243,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1272,7 +1518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10</v>
       </c>
@@ -1301,7 +1547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10</v>
       </c>
@@ -1330,7 +1576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>10</v>
       </c>
@@ -1359,7 +1605,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20</v>
       </c>
@@ -1388,7 +1634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20</v>
       </c>
@@ -1417,7 +1663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20</v>
       </c>
@@ -1446,7 +1692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20</v>
       </c>
@@ -1475,7 +1721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20</v>
       </c>
@@ -1504,7 +1750,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>30</v>
       </c>
@@ -1533,7 +1779,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>30</v>
       </c>
@@ -1562,7 +1808,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>30</v>
       </c>
@@ -1591,7 +1837,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>30</v>
       </c>
@@ -1620,7 +1866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>30</v>
       </c>
@@ -1649,7 +1895,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>40</v>
       </c>
@@ -1678,7 +1924,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>40</v>
       </c>
@@ -1707,7 +1953,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>40</v>
       </c>
@@ -1736,7 +1982,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>40</v>
       </c>
@@ -1765,7 +2011,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>40</v>
       </c>
@@ -1794,7 +2040,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>50</v>
       </c>
@@ -1823,7 +2069,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>50</v>
       </c>
@@ -1852,7 +2098,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>50</v>
       </c>
@@ -1881,7 +2127,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>50</v>
       </c>
@@ -1910,7 +2156,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>50</v>
       </c>
@@ -1939,7 +2185,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>120</v>
       </c>
@@ -1968,7 +2214,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>120</v>
       </c>
@@ -1997,7 +2243,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>120</v>
       </c>
@@ -2026,7 +2272,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>120</v>
       </c>
@@ -2055,7 +2301,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>120</v>
       </c>
@@ -2084,7 +2330,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>150</v>
       </c>
@@ -2113,7 +2359,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>150</v>
       </c>
@@ -2142,7 +2388,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>150</v>
       </c>
@@ -2171,7 +2417,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>150</v>
       </c>
@@ -2200,7 +2446,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>150</v>
       </c>
@@ -2229,7 +2475,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>180</v>
       </c>
@@ -2258,7 +2504,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>180</v>
       </c>
@@ -2287,7 +2533,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>180</v>
       </c>
@@ -2316,7 +2562,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>180</v>
       </c>
@@ -2345,7 +2591,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>180</v>
       </c>
@@ -2374,7 +2620,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>60</v>
       </c>
@@ -2403,7 +2649,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>60</v>
       </c>
@@ -2432,7 +2678,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>60</v>
       </c>
@@ -2461,7 +2707,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>60</v>
       </c>
@@ -2490,7 +2736,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>60</v>
       </c>
@@ -2519,7 +2765,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>90</v>
       </c>
@@ -2548,7 +2794,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>90</v>
       </c>
@@ -2577,7 +2823,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>90</v>
       </c>
@@ -2606,7 +2852,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>90</v>
       </c>
@@ -2635,7 +2881,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>90</v>
       </c>
@@ -2664,7 +2910,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>10</v>
       </c>
@@ -2693,7 +2939,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>10</v>
       </c>
@@ -2722,7 +2968,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>10</v>
       </c>
@@ -2751,7 +2997,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>10</v>
       </c>
@@ -2780,7 +3026,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>10</v>
       </c>
@@ -2809,7 +3055,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>20</v>
       </c>
@@ -2838,7 +3084,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>20</v>
       </c>
@@ -2867,7 +3113,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>20</v>
       </c>
@@ -2896,7 +3142,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>20</v>
       </c>
@@ -2925,7 +3171,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>20</v>
       </c>
@@ -2954,7 +3200,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>30</v>
       </c>
@@ -2983,7 +3229,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>30</v>
       </c>
@@ -3012,7 +3258,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>30</v>
       </c>
@@ -3041,7 +3287,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>30</v>
       </c>
@@ -3070,7 +3316,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>30</v>
       </c>
@@ -3099,7 +3345,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>40</v>
       </c>
@@ -3128,7 +3374,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>40</v>
       </c>
@@ -3157,7 +3403,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>40</v>
       </c>
@@ -3186,7 +3432,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>40</v>
       </c>
@@ -3215,7 +3461,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>40</v>
       </c>
@@ -3244,7 +3490,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>50</v>
       </c>
@@ -3273,7 +3519,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>50</v>
       </c>
@@ -3302,7 +3548,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>50</v>
       </c>
@@ -3331,7 +3577,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>50</v>
       </c>
@@ -3360,7 +3606,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>50</v>
       </c>
@@ -3389,7 +3635,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>100</v>
       </c>
@@ -3418,7 +3664,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>100</v>
       </c>
@@ -3447,7 +3693,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>100</v>
       </c>
@@ -3476,7 +3722,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>100</v>
       </c>
@@ -3505,7 +3751,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>100</v>
       </c>
@@ -3534,7 +3780,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>20</v>
       </c>
@@ -3563,7 +3809,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>20</v>
       </c>
@@ -3592,7 +3838,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>20</v>
       </c>
@@ -3621,7 +3867,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>20</v>
       </c>
@@ -3650,7 +3896,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>20</v>
       </c>
@@ -3679,7 +3925,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>40</v>
       </c>
@@ -3708,7 +3954,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>40</v>
       </c>
@@ -3737,7 +3983,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>40</v>
       </c>
@@ -3766,7 +4012,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>40</v>
       </c>
@@ -3795,7 +4041,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>40</v>
       </c>
@@ -3824,7 +4070,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>60</v>
       </c>
@@ -3853,7 +4099,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>60</v>
       </c>
@@ -3882,7 +4128,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>60</v>
       </c>
@@ -3911,7 +4157,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>60</v>
       </c>
@@ -3940,7 +4186,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>60</v>
       </c>
@@ -3969,7 +4215,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>80</v>
       </c>
@@ -3998,7 +4244,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>80</v>
       </c>
@@ -4027,7 +4273,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>80</v>
       </c>
@@ -4056,7 +4302,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>80</v>
       </c>
@@ -4085,7 +4331,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>80</v>
       </c>
@@ -4120,16 +4366,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>112</v>
       </c>
@@ -4155,654 +4404,654 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>660</v>
+        <v>521</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>0</v>
+      <c r="D2" t="s">
+        <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0.10149681156927701</v>
+        <v>115</v>
+      </c>
+      <c r="F2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" t="s">
+        <v>117</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>658</v>
+        <v>522</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3">
-        <v>0</v>
+      <c r="D3" t="s">
+        <v>119</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>9.8179289215805404E-2</v>
+        <v>120</v>
+      </c>
+      <c r="F3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" t="s">
+        <v>122</v>
       </c>
       <c r="H3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>701</v>
+        <v>494</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>0</v>
+      <c r="D4" t="s">
+        <v>124</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>9.9244661305949E-2</v>
+        <v>120</v>
+      </c>
+      <c r="F4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" t="s">
+        <v>126</v>
       </c>
       <c r="H4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>634</v>
+        <v>530</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>0</v>
+      <c r="D5" t="s">
+        <v>128</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0.10089654483805</v>
+      <c r="F5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" t="s">
+        <v>129</v>
       </c>
       <c r="H5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>626</v>
+        <v>508</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0.30990415335463201</v>
-      </c>
-      <c r="F6">
-        <v>0.51230125607281995</v>
-      </c>
-      <c r="G6">
-        <v>0.100173188453968</v>
-      </c>
-      <c r="H6">
-        <v>2.33892450618556E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20</v>
       </c>
       <c r="B7">
-        <v>674</v>
+        <v>542</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7">
-        <v>0</v>
+      <c r="D7" t="s">
+        <v>134</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>9.94117020905044E-2</v>
+        <v>135</v>
+      </c>
+      <c r="F7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G7" t="s">
+        <v>137</v>
       </c>
       <c r="H7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20</v>
       </c>
       <c r="B8">
-        <v>676</v>
+        <v>524</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8">
-        <v>0</v>
+      <c r="D8" t="s">
+        <v>139</v>
       </c>
       <c r="E8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0.100615577723122</v>
+        <v>120</v>
+      </c>
+      <c r="F8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G8" t="s">
+        <v>141</v>
       </c>
       <c r="H8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20</v>
       </c>
       <c r="B9">
-        <v>679</v>
+        <v>497</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9">
-        <v>0</v>
+      <c r="D9" t="s">
+        <v>128</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>9.9859972986822795E-2</v>
+      <c r="F9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" t="s">
+        <v>143</v>
       </c>
       <c r="H9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20</v>
       </c>
       <c r="B10">
-        <v>685</v>
+        <v>504</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
-      <c r="D10">
-        <v>0</v>
+      <c r="D10" t="s">
+        <v>128</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0.10185868297525399</v>
+      <c r="F10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" t="s">
+        <v>144</v>
       </c>
       <c r="H10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20</v>
       </c>
       <c r="B11">
-        <v>644</v>
+        <v>518</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>0.32919254658385</v>
-      </c>
-      <c r="F11">
-        <v>0.52813388838487896</v>
-      </c>
-      <c r="G11">
-        <v>9.7548789675384606E-2</v>
-      </c>
-      <c r="H11">
-        <v>2.21123419528301E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" t="s">
+        <v>145</v>
+      </c>
+      <c r="F11" t="s">
+        <v>146</v>
+      </c>
+      <c r="G11" t="s">
+        <v>147</v>
+      </c>
+      <c r="H11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B12">
-        <v>666</v>
+        <v>529</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12">
-        <v>0</v>
+      <c r="D12" t="s">
+        <v>149</v>
       </c>
       <c r="E12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0.100149929050822</v>
+        <v>150</v>
+      </c>
+      <c r="F12" t="s">
+        <v>151</v>
+      </c>
+      <c r="G12" t="s">
+        <v>152</v>
       </c>
       <c r="H12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B13">
-        <v>655</v>
+        <v>506</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13">
-        <v>0</v>
+      <c r="D13" t="s">
+        <v>154</v>
       </c>
       <c r="E13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>9.7579100468797503E-2</v>
+        <v>120</v>
+      </c>
+      <c r="F13" t="s">
+        <v>155</v>
+      </c>
+      <c r="G13" t="s">
+        <v>156</v>
       </c>
       <c r="H13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B14">
-        <v>654</v>
+        <v>516</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
-      <c r="D14">
-        <v>0</v>
+      <c r="D14" t="s">
+        <v>158</v>
       </c>
       <c r="E14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>9.8871449567073097E-2</v>
+        <v>120</v>
+      </c>
+      <c r="F14" t="s">
+        <v>159</v>
+      </c>
+      <c r="G14" t="s">
+        <v>160</v>
       </c>
       <c r="H14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B15">
-        <v>657</v>
+        <v>508</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
-      <c r="D15">
-        <v>0</v>
+      <c r="D15" t="s">
+        <v>128</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0.10413952737234</v>
+      <c r="F15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G15" t="s">
+        <v>162</v>
       </c>
       <c r="H15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B16">
-        <v>639</v>
+        <v>545</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>0.34272300469483502</v>
-      </c>
-      <c r="F16">
-        <v>0.52377143319972097</v>
-      </c>
-      <c r="G16">
-        <v>9.8109288842923706E-2</v>
-      </c>
-      <c r="H16">
-        <v>2.3759181680365199E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" t="s">
+        <v>163</v>
+      </c>
+      <c r="F16" t="s">
+        <v>164</v>
+      </c>
+      <c r="G16" t="s">
+        <v>165</v>
+      </c>
+      <c r="H16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B17">
-        <v>665</v>
+        <v>528</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17">
-        <v>0</v>
+      <c r="D17" t="s">
+        <v>167</v>
       </c>
       <c r="E17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0.10028630653153101</v>
+        <v>120</v>
+      </c>
+      <c r="F17" t="s">
+        <v>168</v>
+      </c>
+      <c r="G17" t="s">
+        <v>169</v>
       </c>
       <c r="H17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B18">
-        <v>637</v>
+        <v>503</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="D18">
-        <v>0</v>
+      <c r="D18" t="s">
+        <v>171</v>
       </c>
       <c r="E18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0.10151934056651001</v>
+        <v>120</v>
+      </c>
+      <c r="F18" t="s">
+        <v>172</v>
+      </c>
+      <c r="G18" t="s">
+        <v>173</v>
       </c>
       <c r="H18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B19">
-        <v>699</v>
+        <v>506</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
-      <c r="D19">
-        <v>0</v>
+      <c r="D19" t="s">
+        <v>128</v>
       </c>
       <c r="E19" t="s">
         <v>2</v>
       </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0.100095102701428</v>
+      <c r="F19" t="s">
+        <v>128</v>
+      </c>
+      <c r="G19" t="s">
+        <v>175</v>
       </c>
       <c r="H19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B20">
-        <v>661</v>
+        <v>490</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
-      <c r="D20">
-        <v>0</v>
+      <c r="D20" t="s">
+        <v>128</v>
       </c>
       <c r="E20" t="s">
         <v>2</v>
       </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>9.7220314751131201E-2</v>
+      <c r="F20" t="s">
+        <v>128</v>
+      </c>
+      <c r="G20" t="s">
+        <v>176</v>
       </c>
       <c r="H20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B21">
-        <v>659</v>
+        <v>494</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>0.29742033383915001</v>
-      </c>
-      <c r="F21">
-        <v>0.53985741098389906</v>
-      </c>
-      <c r="G21">
-        <v>9.9188970767722401E-2</v>
-      </c>
-      <c r="H21">
-        <v>2.4227512790816301E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" t="s">
+        <v>177</v>
+      </c>
+      <c r="F21" t="s">
+        <v>178</v>
+      </c>
+      <c r="G21" t="s">
+        <v>179</v>
+      </c>
+      <c r="H21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="B22">
-        <v>640</v>
+        <v>535</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22">
-        <v>0</v>
+      <c r="D22" t="s">
+        <v>181</v>
       </c>
       <c r="E22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0.10158857972897101</v>
+        <v>182</v>
+      </c>
+      <c r="F22" t="s">
+        <v>183</v>
+      </c>
+      <c r="G22" t="s">
+        <v>184</v>
       </c>
       <c r="H22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="B23">
-        <v>672</v>
+        <v>496</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
-      <c r="D23">
-        <v>0</v>
+      <c r="D23" t="s">
+        <v>186</v>
       </c>
       <c r="E23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0.10222176945170799</v>
+        <v>120</v>
+      </c>
+      <c r="F23" t="s">
+        <v>187</v>
+      </c>
+      <c r="G23" t="s">
+        <v>188</v>
       </c>
       <c r="H23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="B24">
-        <v>695</v>
+        <v>497</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
-      <c r="D24">
-        <v>0</v>
+      <c r="D24" t="s">
+        <v>128</v>
       </c>
       <c r="E24" t="s">
         <v>2</v>
       </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0.100518011932761</v>
+      <c r="F24" t="s">
+        <v>128</v>
+      </c>
+      <c r="G24" t="s">
+        <v>190</v>
       </c>
       <c r="H24" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="B25">
-        <v>667</v>
+        <v>498</v>
       </c>
       <c r="C25">
         <v>4</v>
       </c>
-      <c r="D25">
-        <v>0</v>
+      <c r="D25" t="s">
+        <v>128</v>
       </c>
       <c r="E25" t="s">
         <v>2</v>
       </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0.100997419414306</v>
+      <c r="F25" t="s">
+        <v>128</v>
+      </c>
+      <c r="G25" t="s">
+        <v>191</v>
       </c>
       <c r="H25" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="B26">
-        <v>607</v>
+        <v>548</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>0.24382207578253701</v>
-      </c>
-      <c r="F26">
-        <v>0.49662609270299601</v>
-      </c>
-      <c r="G26">
-        <v>9.8741838909983601E-2</v>
-      </c>
-      <c r="H26">
-        <v>2.21242575067567E-2</v>
+      <c r="D26" t="s">
+        <v>120</v>
+      </c>
+      <c r="E26" t="s">
+        <v>192</v>
+      </c>
+      <c r="F26" t="s">
+        <v>193</v>
+      </c>
+      <c r="G26" t="s">
+        <v>194</v>
+      </c>
+      <c r="H26" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -4811,16 +5060,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -4846,7 +5095,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -4872,7 +5121,7 @@
         <v>5.3454431954773798E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10</v>
       </c>
@@ -4898,7 +5147,7 @@
         <v>7.6772648499999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10</v>
       </c>
@@ -4924,7 +5173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>10</v>
       </c>
@@ -4950,7 +5199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>10</v>
       </c>
@@ -4976,7 +5225,7 @@
         <v>4.1514522431535202E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20</v>
       </c>
@@ -5002,7 +5251,7 @@
         <v>5.5624055779005498E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20</v>
       </c>
@@ -5028,7 +5277,7 @@
         <v>8.4897546529411699E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20</v>
       </c>
@@ -5054,7 +5303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20</v>
       </c>
@@ -5080,7 +5329,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20</v>
       </c>
@@ -5106,7 +5355,7 @@
         <v>4.2254844710659899E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>30</v>
       </c>
@@ -5132,7 +5381,7 @@
         <v>5.5861443811203303E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>30</v>
       </c>
@@ -5158,7 +5407,7 @@
         <v>8.9561662258064501E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>30</v>
       </c>
@@ -5184,7 +5433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>30</v>
       </c>
@@ -5210,7 +5459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>30</v>
       </c>
@@ -5236,7 +5485,7 @@
         <v>3.72664187107438E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>40</v>
       </c>
@@ -5262,7 +5511,7 @@
         <v>5.4226535323580002E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>40</v>
       </c>
@@ -5288,7 +5537,7 @@
         <v>8.9503700085365803E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>40</v>
       </c>
@@ -5314,7 +5563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>40</v>
       </c>
@@ -5340,7 +5589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>40</v>
       </c>
@@ -5366,7 +5615,7 @@
         <v>3.7863600859649099E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>50</v>
       </c>
@@ -5392,7 +5641,7 @@
         <v>5.3313234756834499E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>50</v>
       </c>
@@ -5418,7 +5667,7 @@
         <v>9.0546043287878797E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>50</v>
       </c>
@@ -5444,7 +5693,7 @@
         <v>0.114976783</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>50</v>
       </c>
@@ -5470,7 +5719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>50</v>
       </c>
@@ -5502,20 +5751,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>110</v>
       </c>
@@ -5541,7 +5790,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>120</v>
       </c>
@@ -5567,7 +5816,7 @@
         <v>6.7192155084459401E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>120</v>
       </c>
@@ -5593,7 +5842,7 @@
         <v>9.5940830732142796E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>120</v>
       </c>
@@ -5619,7 +5868,7 @@
         <v>0.10663840902777701</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>120</v>
       </c>
@@ -5645,7 +5894,7 @@
         <v>0.1186932798125</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>120</v>
       </c>
@@ -5671,7 +5920,7 @@
         <v>4.7460517422121901E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>150</v>
       </c>
@@ -5697,7 +5946,7 @@
         <v>9.4745911634304195E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>150</v>
       </c>
@@ -5723,7 +5972,7 @@
         <v>0.115885011571428</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>150</v>
       </c>
@@ -5749,7 +5998,7 @@
         <v>0.13344005501923001</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>150</v>
       </c>
@@ -5775,7 +6024,7 @@
         <v>0.15727358012499901</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>150</v>
       </c>
@@ -5801,7 +6050,7 @@
         <v>8.2472841082191703E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>180</v>
       </c>
@@ -5827,7 +6076,7 @@
         <v>0.1173843044009</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>180</v>
       </c>
@@ -5853,7 +6102,7 @@
         <v>0.14290281706794</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>180</v>
       </c>
@@ -5879,7 +6128,7 @@
         <v>0.16968063013736201</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>180</v>
       </c>
@@ -5905,7 +6154,7 @@
         <v>0.16956124622222199</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>180</v>
       </c>
@@ -5931,7 +6180,7 @@
         <v>9.2829002143750006E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>60</v>
       </c>
@@ -5957,7 +6206,7 @@
         <v>2.1980603588235201E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>60</v>
       </c>
@@ -5983,7 +6232,7 @@
         <v>3.62149924E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>60</v>
       </c>
@@ -6009,7 +6258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>60</v>
       </c>
@@ -6035,7 +6284,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>60</v>
       </c>
@@ -6061,7 +6310,7 @@
         <v>1.3267227649999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>90</v>
       </c>
@@ -6087,7 +6336,7 @@
         <v>4.92132457742782E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>90</v>
       </c>
@@ -6113,7 +6362,7 @@
         <v>6.6859150377049106E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>90</v>
       </c>
@@ -6139,7 +6388,7 @@
         <v>8.2416933375000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>90</v>
       </c>
@@ -6165,7 +6414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>90</v>
       </c>
@@ -6197,22 +6446,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>102</v>
       </c>
@@ -6238,7 +6487,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -6264,7 +6513,7 @@
         <v>5.3474230869565202E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10</v>
       </c>
@@ -6290,7 +6539,7 @@
         <v>8.2439300666666604E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10</v>
       </c>
@@ -6316,7 +6565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>10</v>
       </c>
@@ -6342,7 +6591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>10</v>
       </c>
@@ -6368,7 +6617,7 @@
         <v>4.2008497092592502E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20</v>
       </c>
@@ -6394,7 +6643,7 @@
         <v>5.0666469828715303E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20</v>
       </c>
@@ -6420,7 +6669,7 @@
         <v>8.0597526107142797E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20</v>
       </c>
@@ -6446,7 +6695,7 @@
         <v>0.10420987399999999</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20</v>
       </c>
@@ -6472,7 +6721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20</v>
       </c>
@@ -6498,7 +6747,7 @@
         <v>4.3132122662280697E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>30</v>
       </c>
@@ -6524,7 +6773,7 @@
         <v>5.1250953008590998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>30</v>
       </c>
@@ -6550,7 +6799,7 @@
         <v>8.0871005388888806E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>30</v>
       </c>
@@ -6576,7 +6825,7 @@
         <v>0.12002144200000001</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>30</v>
       </c>
@@ -6602,7 +6851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>30</v>
       </c>
@@ -6628,7 +6877,7 @@
         <v>3.4365185409207098E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>40</v>
       </c>
@@ -6654,7 +6903,7 @@
         <v>5.1401913727793597E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>40</v>
       </c>
@@ -6680,7 +6929,7 @@
         <v>7.8710458406014996E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>40</v>
       </c>
@@ -6706,7 +6955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>40</v>
       </c>
@@ -6732,7 +6981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>40</v>
       </c>
@@ -6758,7 +7007,7 @@
         <v>3.3010532216535403E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>50</v>
       </c>
@@ -6784,7 +7033,7 @@
         <v>4.8722617259627302E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>50</v>
       </c>
@@ -6810,7 +7059,7 @@
         <v>8.0342337420634902E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>50</v>
       </c>
@@ -6836,7 +7085,7 @@
         <v>0.1238634062</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>50</v>
       </c>
@@ -6862,7 +7111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>50</v>
       </c>

</xml_diff>